<commit_message>
modified district names to be compatible with the visualisation
</commit_message>
<xml_diff>
--- a/data/population_dataset.xlsx
+++ b/data/population_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ines/Documents/Studium/Master/DataLiteracy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannaheiss/Desktop/DataLiteracy/Data-Literacy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95CD8FA-2CE0-D843-B647-B91D34D07087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519086AE-7CF5-7640-AB16-EA0C072B6D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28280" windowHeight="16260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="28280" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deckblatt" sheetId="1" r:id="rId1"/>
@@ -4745,91 +4745,91 @@
       <c r="A12" s="48"/>
       <c r="H12" s="48"/>
     </row>
-    <row r="13" spans="1:11" ht="14">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="40"/>
       <c r="D13" s="47"/>
     </row>
-    <row r="14" spans="1:11" ht="14">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="40"/>
       <c r="D14" s="47"/>
     </row>
-    <row r="15" spans="1:11" ht="14">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="40"/>
       <c r="D15" s="47"/>
     </row>
-    <row r="16" spans="1:11" ht="14">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="40"/>
       <c r="D16" s="47"/>
     </row>
-    <row r="17" spans="1:4" ht="14">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="40"/>
       <c r="D17" s="47"/>
     </row>
-    <row r="18" spans="1:4" ht="14">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="40"/>
       <c r="D18" s="47"/>
     </row>
-    <row r="19" spans="1:4" ht="14">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="40"/>
       <c r="D19" s="47"/>
     </row>
-    <row r="20" spans="1:4" ht="14">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="40"/>
       <c r="D20" s="47"/>
     </row>
-    <row r="21" spans="1:4" ht="14">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="40"/>
       <c r="D21" s="47"/>
     </row>
-    <row r="22" spans="1:4" ht="14">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="40"/>
       <c r="D22" s="47"/>
     </row>
-    <row r="23" spans="1:4" ht="14">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="40"/>
       <c r="D23" s="47"/>
     </row>
-    <row r="24" spans="1:4" ht="14">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="40"/>
       <c r="D24" s="47"/>
     </row>
-    <row r="25" spans="1:4" ht="14">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="40"/>
       <c r="D25" s="47"/>
     </row>
-    <row r="26" spans="1:4" ht="14">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="40"/>
       <c r="D26" s="47"/>
     </row>
-    <row r="27" spans="1:4" ht="14">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="40"/>
       <c r="D27" s="47"/>
     </row>
-    <row r="28" spans="1:4" ht="14">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="40"/>
       <c r="D28" s="47"/>
     </row>
-    <row r="29" spans="1:4" ht="14">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" s="40"/>
       <c r="D29" s="47"/>
     </row>
-    <row r="30" spans="1:4" ht="14">
+    <row r="30" spans="1:4" ht="15">
       <c r="A30" s="40"/>
       <c r="D30" s="47"/>
     </row>
-    <row r="31" spans="1:4" ht="14">
+    <row r="31" spans="1:4" ht="15">
       <c r="A31" s="40"/>
       <c r="D31" s="47"/>
     </row>
-    <row r="32" spans="1:4" ht="14">
+    <row r="32" spans="1:4" ht="15">
       <c r="A32" s="40"/>
       <c r="D32" s="47"/>
     </row>
-    <row r="33" spans="1:11" ht="14">
+    <row r="33" spans="1:11" ht="15">
       <c r="A33" s="40"/>
       <c r="D33" s="47"/>
     </row>
-    <row r="34" spans="1:11" ht="25">
+    <row r="34" spans="1:11" ht="26">
       <c r="A34" s="48" t="s">
         <v>1308</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="14">
+    <row r="36" spans="1:11" ht="15">
       <c r="A36" s="40"/>
     </row>
     <row r="38" spans="1:11">
@@ -4901,8 +4901,8 @@
   <dimension ref="A1:M648"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="2" topLeftCell="A353" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B370" sqref="B370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -5460,7 +5460,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1">
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="15">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -5949,7 +5949,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" ht="15">
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="11"/>
@@ -5958,7 +5958,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" ht="15">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" ht="15">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>2467</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" ht="15">
       <c r="A22" s="3" t="s">
         <v>60</v>
       </c>
@@ -6023,7 +6023,7 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" ht="15">
       <c r="A23" s="22" t="s">
         <v>62</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="15">
       <c r="A34" s="22" t="s">
         <v>94</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="15">
       <c r="A42" s="22" t="s">
         <v>117</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" ht="15">
       <c r="A54" s="22" t="s">
         <v>152</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" ht="15">
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
       <c r="D72" s="11"/>
@@ -7254,7 +7254,7 @@
       <c r="G72" s="12"/>
       <c r="H72" s="12"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" ht="15">
       <c r="A73" s="3" t="s">
         <v>205</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" ht="15">
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
@@ -7339,7 +7339,7 @@
       <c r="G76" s="12"/>
       <c r="H76" s="12"/>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" ht="15">
       <c r="A77" s="3" t="s">
         <v>213</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" ht="15">
       <c r="A78" s="3" t="s">
         <v>215</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" ht="15">
       <c r="A94" s="3" t="s">
         <v>262</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" ht="15">
       <c r="A106" s="3" t="s">
         <v>297</v>
       </c>
@@ -8286,7 +8286,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" ht="15">
       <c r="A115" s="3" t="s">
         <v>323</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" ht="15">
       <c r="A123" s="3" t="s">
         <v>346</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" ht="15">
       <c r="B136" s="9"/>
       <c r="C136" s="10"/>
       <c r="D136" s="11"/>
@@ -8816,7 +8816,7 @@
       <c r="G136" s="12"/>
       <c r="H136" s="12"/>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" ht="15">
       <c r="A137" s="3" t="s">
         <v>384</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" ht="15">
       <c r="A138" s="3" t="s">
         <v>386</v>
       </c>
@@ -9217,7 +9217,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" ht="15">
       <c r="A153" s="3" t="s">
         <v>430</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" ht="15">
       <c r="A159" s="3" t="s">
         <v>447</v>
       </c>
@@ -9555,7 +9555,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" ht="15">
       <c r="B167" s="9"/>
       <c r="C167" s="10"/>
       <c r="D167" s="11"/>
@@ -9564,7 +9564,7 @@
       <c r="G167" s="12"/>
       <c r="H167" s="12"/>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" ht="15">
       <c r="A168" s="3" t="s">
         <v>470</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" ht="15">
       <c r="A169" s="22" t="s">
         <v>472</v>
       </c>
@@ -9887,7 +9887,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" ht="15">
       <c r="A181" s="22" t="s">
         <v>507</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" ht="15">
       <c r="A187" s="22" t="s">
         <v>524</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" ht="15">
       <c r="B208" s="9"/>
       <c r="C208" s="10"/>
       <c r="D208" s="11"/>
@@ -10572,7 +10572,7 @@
       <c r="G208" s="12"/>
       <c r="H208" s="12"/>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" ht="15">
       <c r="A209" s="3" t="s">
         <v>586</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" ht="15">
       <c r="A210" s="3" t="s">
         <v>588</v>
       </c>
@@ -10608,7 +10608,7 @@
       <c r="G210" s="21"/>
       <c r="H210" s="21"/>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" ht="15">
       <c r="A211" s="3" t="s">
         <v>590</v>
       </c>
@@ -10777,7 +10777,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" ht="15">
       <c r="A218" s="3" t="s">
         <v>610</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" ht="15">
       <c r="A224" s="3" t="s">
         <v>627</v>
       </c>
@@ -10985,7 +10985,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" ht="15">
       <c r="A227" s="3" t="s">
         <v>635</v>
       </c>
@@ -10998,7 +10998,7 @@
       <c r="G227" s="21"/>
       <c r="H227" s="21"/>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" ht="15">
       <c r="A228" s="3" t="s">
         <v>637</v>
       </c>
@@ -11119,7 +11119,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" ht="15">
       <c r="A233" s="3" t="s">
         <v>652</v>
       </c>
@@ -11240,7 +11240,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" ht="15">
       <c r="A238" s="3" t="s">
         <v>666</v>
       </c>
@@ -11359,7 +11359,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" ht="15">
       <c r="A243" s="3" t="s">
         <v>680</v>
       </c>
@@ -11372,7 +11372,7 @@
       <c r="G243" s="21"/>
       <c r="H243" s="21"/>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" ht="15">
       <c r="A244" s="3" t="s">
         <v>682</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" ht="15">
       <c r="A249" s="3" t="s">
         <v>696</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" ht="15">
       <c r="A253" s="3" t="s">
         <v>707</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" ht="15">
       <c r="A257" s="3" t="s">
         <v>718</v>
       </c>
@@ -11692,7 +11692,7 @@
       <c r="G257" s="21"/>
       <c r="H257" s="21"/>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" ht="15">
       <c r="A258" s="3" t="s">
         <v>720</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" ht="15">
       <c r="A262" s="3" t="s">
         <v>731</v>
       </c>
@@ -11882,7 +11882,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" ht="15">
       <c r="A266" s="3" t="s">
         <v>742</v>
       </c>
@@ -11978,7 +11978,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" ht="15">
       <c r="B270" s="9"/>
       <c r="C270" s="10"/>
       <c r="D270" s="11"/>
@@ -11987,7 +11987,7 @@
       <c r="G270" s="12"/>
       <c r="H270" s="12"/>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" ht="15">
       <c r="A271" s="3" t="s">
         <v>753</v>
       </c>
@@ -12011,7 +12011,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" ht="15">
       <c r="A272" s="3" t="s">
         <v>755</v>
       </c>
@@ -12622,7 +12622,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" ht="15">
       <c r="A296" s="3" t="s">
         <v>825</v>
       </c>
@@ -12947,7 +12947,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" ht="15">
       <c r="A309" s="3" t="s">
         <v>861</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" ht="15">
       <c r="A320" s="3" t="s">
         <v>892</v>
       </c>
@@ -13571,7 +13571,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:8" ht="15">
       <c r="A334" s="3" t="s">
         <v>929</v>
       </c>
@@ -13899,7 +13899,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:8" ht="15">
       <c r="A347" s="3" t="s">
         <v>965</v>
       </c>
@@ -14227,7 +14227,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="360" spans="1:8">
+    <row r="360" spans="1:8" ht="15">
       <c r="A360" s="3" t="s">
         <v>1000</v>
       </c>
@@ -14607,7 +14607,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" ht="15">
       <c r="B375" s="9"/>
       <c r="C375" s="10"/>
       <c r="D375" s="11"/>
@@ -14616,7 +14616,7 @@
       <c r="G375" s="12"/>
       <c r="H375" s="12"/>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" ht="15">
       <c r="A376" s="3" t="s">
         <v>1043</v>
       </c>
@@ -14796,7 +14796,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" ht="15">
       <c r="B383" s="9"/>
       <c r="C383" s="10"/>
       <c r="D383" s="11"/>
@@ -14805,7 +14805,7 @@
       <c r="G383" s="12"/>
       <c r="H383" s="12"/>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" ht="15">
       <c r="A384" s="3" t="s">
         <v>1063</v>
       </c>
@@ -14829,7 +14829,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" ht="15">
       <c r="A385" s="4" t="s">
         <v>1065</v>
       </c>
@@ -14855,7 +14855,7 @@
         <v>4136</v>
       </c>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" ht="15">
       <c r="A386" s="3" t="s">
         <v>1068</v>
       </c>
@@ -15336,7 +15336,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="405" spans="1:8">
+    <row r="405" spans="1:8" ht="15">
       <c r="B405" s="9"/>
       <c r="C405" s="10"/>
       <c r="D405" s="11"/>
@@ -15345,7 +15345,7 @@
       <c r="G405" s="12"/>
       <c r="H405" s="12"/>
     </row>
-    <row r="406" spans="1:8">
+    <row r="406" spans="1:8" ht="15">
       <c r="A406" s="3" t="s">
         <v>1124</v>
       </c>
@@ -15577,7 +15577,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="415" spans="1:8">
+    <row r="415" spans="1:8" ht="15">
       <c r="B415" s="9"/>
       <c r="C415" s="10"/>
       <c r="D415" s="11"/>
@@ -15586,7 +15586,7 @@
       <c r="G415" s="12"/>
       <c r="H415" s="12"/>
     </row>
-    <row r="416" spans="1:8">
+    <row r="416" spans="1:8" ht="15">
       <c r="A416" s="3" t="s">
         <v>1150</v>
       </c>
@@ -15610,7 +15610,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="417" spans="1:8">
+    <row r="417" spans="1:8" ht="15">
       <c r="A417" s="18">
         <v>145</v>
       </c>
@@ -15753,7 +15753,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="423" spans="1:8">
+    <row r="423" spans="1:8" ht="15">
       <c r="A423" s="18">
         <v>146</v>
       </c>
@@ -15896,7 +15896,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="429" spans="1:8">
+    <row r="429" spans="1:8" ht="15">
       <c r="A429" s="18">
         <v>147</v>
       </c>
@@ -15987,7 +15987,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="433" spans="1:8">
+    <row r="433" spans="1:8" ht="15">
       <c r="B433" s="9"/>
       <c r="C433" s="10"/>
       <c r="D433" s="11"/>
@@ -15996,7 +15996,7 @@
       <c r="G433" s="12"/>
       <c r="H433" s="12"/>
     </row>
-    <row r="434" spans="1:8">
+    <row r="434" spans="1:8" ht="15">
       <c r="A434" s="3" t="s">
         <v>1191</v>
       </c>
@@ -16384,7 +16384,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="449" spans="1:8">
+    <row r="449" spans="1:8" ht="15">
       <c r="B449" s="9"/>
       <c r="C449" s="10"/>
       <c r="D449" s="11"/>
@@ -16393,7 +16393,7 @@
       <c r="G449" s="12"/>
       <c r="H449" s="12"/>
     </row>
-    <row r="450" spans="1:8">
+    <row r="450" spans="1:8" ht="15">
       <c r="A450" s="3" t="s">
         <v>1235</v>
       </c>
@@ -16989,7 +16989,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="473" spans="1:8">
+    <row r="473" spans="1:8" ht="15">
       <c r="B473" s="9"/>
       <c r="C473" s="10"/>
       <c r="D473" s="11"/>
@@ -17075,7 +17075,7 @@
       <c r="G479" s="4"/>
       <c r="H479" s="4"/>
     </row>
-    <row r="480" spans="1:8">
+    <row r="480" spans="1:8" ht="15">
       <c r="A480" s="17"/>
       <c r="B480" s="37"/>
       <c r="C480" s="37"/>
@@ -17085,7 +17085,7 @@
       <c r="G480" s="39"/>
       <c r="H480" s="4"/>
     </row>
-    <row r="481" spans="1:8">
+    <row r="481" spans="1:8" ht="15">
       <c r="A481" s="40" t="s">
         <v>5</v>
       </c>
@@ -17097,7 +17097,7 @@
       <c r="G481" s="40"/>
       <c r="H481" s="40"/>
     </row>
-    <row r="482" spans="1:8">
+    <row r="482" spans="1:8" ht="15">
       <c r="A482" s="40" t="s">
         <v>1309</v>
       </c>
@@ -17109,7 +17109,7 @@
       <c r="G482" s="40"/>
       <c r="H482" s="40"/>
     </row>
-    <row r="483" spans="1:8">
+    <row r="483" spans="1:8" ht="15">
       <c r="A483" s="40" t="s">
         <v>6</v>
       </c>

</xml_diff>